<commit_message>
Updated database to spell out mm and ucm
</commit_message>
<xml_diff>
--- a/resources/db/Case_Types.xlsx
+++ b/resources/db/Case_Types.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python39\MuniEntry\resources\db\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA2E546-A976-42EA-90ED-48E683C3313C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9A2A0F97-FC7F-AD45-9789-0CD0F1FECE89}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,18 +81,12 @@
     <t>4511.20</t>
   </si>
   <si>
-    <t>MM</t>
-  </si>
-  <si>
     <t>Wrongful Entrustment of Motor Vehicle</t>
   </si>
   <si>
     <t>4511.203</t>
   </si>
   <si>
-    <t>UCM</t>
-  </si>
-  <si>
     <t>Discretionary Class 7 OL suspension; Discretionary immobilization for 30 days if the vehicle used is registered to D</t>
   </si>
   <si>
@@ -259,12 +247,18 @@
   </si>
   <si>
     <t>M1</t>
+  </si>
+  <si>
+    <t>Minor Misdemeanor</t>
+  </si>
+  <si>
+    <t>Unclassified Misdemeanor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -626,28 +620,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C445906-A86A-1E49-AF62-F6D78913993E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,10 +656,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -672,35 +667,35 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -708,101 +703,101 @@
         <v>4511.21</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -810,60 +805,60 @@
         <v>4511.33</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -871,180 +866,180 @@
         <v>4513.04</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K23">
+  <sortState ref="A2:K23">
     <sortCondition ref="B2:B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sorted DB alpha and num added judge full name.
</commit_message>
<xml_diff>
--- a/resources/db/Case_Types.xlsx
+++ b/resources/db/Case_Types.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Child Restraint</t>
   </si>
   <si>
-    <t>Marked Lanes</t>
-  </si>
-  <si>
     <t>Traffic Control Device</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>4511.39</t>
   </si>
   <si>
-    <t>Failure to Stop for  School Bus</t>
-  </si>
-  <si>
     <t>$500 fine; discretionary class 7 suspension of OL (licensed must be delivered to the court who forwards it to the BMV)</t>
   </si>
   <si>
@@ -253,13 +247,22 @@
   </si>
   <si>
     <t>Unclassified Misdemeanor</t>
+  </si>
+  <si>
+    <t>Failure to Stop for School Bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4511.36 </t>
+  </si>
+  <si>
+    <t>If, within one year of the offense, the offender previously has been convicted of or pleaded guilty to one predicate motor vehicle or traffic offense, whoever violates this section is guilty of a misdemeanor of the fourth degree. If, within one year of the offense, the offender previously has been convicted of two or more predicate motor vehicle or traffic offenses, whoever violates this section is guilty of a misdemeanor of the third degree.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +277,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -302,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -314,6 +323,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,21 +638,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.4140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,396 +662,394 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5">
+        <v>4513.04</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4511.21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
-        <v>4511.21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="5">
-        <v>4511.33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5">
-        <v>4513.04</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" t="s">
-        <v>73</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K23">
-    <sortCondition ref="B2:B23"/>
+  <sortState ref="A2:D34">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed failing MMD test due to spacing in offense.
</commit_message>
<xml_diff>
--- a/resources/db/Case_Types.xlsx
+++ b/resources/db/Case_Types.xlsx
@@ -216,9 +216,6 @@
     <t>4511.21(B)(1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Speeding &gt; 25 mph </t>
-  </si>
-  <si>
     <t>4511.21(B)(2)</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>If, within one year of the offense, the offender previously has been convicted of or pleaded guilty to one predicate motor vehicle or traffic offense, whoever violates this section is guilty of a misdemeanor of the fourth degree. If, within one year of the offense, the offender previously has been convicted of two or more predicate motor vehicle or traffic offenses, whoever violates this section is guilty of a misdemeanor of the third degree.</t>
+  </si>
+  <si>
+    <t>Speeding &gt; 25 mph</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -641,18 +641,18 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.4140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.38671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +669,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -677,10 +677,10 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -688,13 +688,13 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -702,10 +702,10 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -713,24 +713,24 @@
         <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -738,21 +738,21 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -760,13 +760,13 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -774,24 +774,24 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -799,10 +799,10 @@
         <v>4513.04</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -810,10 +810,10 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -821,10 +821,10 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -832,10 +832,10 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -843,10 +843,10 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -854,10 +854,10 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -865,10 +865,10 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -876,10 +876,10 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -887,13 +887,13 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -901,13 +901,13 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -915,10 +915,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -926,10 +926,10 @@
         <v>4511.21</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -937,32 +937,32 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -970,10 +970,10 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -981,10 +981,10 @@
         <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -992,24 +992,24 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1017,10 +1017,10 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1028,10 +1028,10 @@
         <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Update charges DB to fix capitalization
</commit_message>
<xml_diff>
--- a/resources/db/Case_Types.xlsx
+++ b/resources/db/Case_Types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python39\MuniEntry\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BFF5AB-EC5A-4D98-9725-913852261155}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22601BD-6E28-498A-B2AF-2757D725F548}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>fine between $25 and $75</t>
   </si>
   <si>
-    <t>Driving under financial responsibility law suspension</t>
-  </si>
-  <si>
     <t>4510.16</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>4510.12(C)(1)</t>
+  </si>
+  <si>
+    <t>Driving Under Financial Responsibility Law Suspension</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -683,10 +683,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -705,71 +705,71 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" t="s">
         <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -788,24 +788,24 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
@@ -819,7 +819,7 @@
         <v>4513.04</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -852,40 +852,40 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,21 +893,21 @@
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>36</v>
@@ -915,13 +915,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>37</v>
@@ -935,7 +935,7 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,40 +946,40 @@
         <v>4511.21</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,10 +998,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,13 +1020,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,10 +1045,10 @@
         <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1059,7 @@
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Adding court costs - still in progress.
</commit_message>
<xml_diff>
--- a/resources/db/Case_Types.xlsx
+++ b/resources/db/Case_Types.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python39\MuniEntry\resources\db\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22601BD-6E28-498A-B2AF-2757D725F548}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
   <si>
     <t>Name of Offense</t>
   </si>
@@ -265,12 +259,24 @@
   </si>
   <si>
     <t>Driving Under Financial Responsibility Law Suspension</t>
+  </si>
+  <si>
+    <t>Offense Type</t>
+  </si>
+  <si>
+    <t>Moving Traffic</t>
+  </si>
+  <si>
+    <t>Non-moving Traffic</t>
+  </si>
+  <si>
+    <t>Criminal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -639,29 +645,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.38671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.38671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.38671875" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,13 +679,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -688,8 +698,11 @@
       <c r="C2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -700,10 +713,13 @@
         <v>69</v>
       </c>
       <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -713,8 +729,11 @@
       <c r="C4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -725,10 +744,13 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -738,8 +760,11 @@
       <c r="C6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -749,8 +774,11 @@
       <c r="C7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -760,8 +788,11 @@
       <c r="C8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -771,8 +802,11 @@
       <c r="C9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -783,10 +817,13 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -796,8 +833,11 @@
       <c r="C11" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -808,10 +848,13 @@
         <v>70</v>
       </c>
       <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -821,8 +864,11 @@
       <c r="C13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -832,8 +878,11 @@
       <c r="C14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -843,8 +892,11 @@
       <c r="C15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -854,8 +906,11 @@
       <c r="C16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -865,8 +920,11 @@
       <c r="C17" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -876,8 +934,11 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -887,8 +948,11 @@
       <c r="C19" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -898,8 +962,11 @@
       <c r="C20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -909,11 +976,14 @@
       <c r="C21" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -923,11 +993,14 @@
       <c r="C22" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -937,8 +1010,11 @@
       <c r="C23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -948,8 +1024,11 @@
       <c r="C24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -959,8 +1038,11 @@
       <c r="C25" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -970,8 +1052,11 @@
       <c r="C26" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -981,8 +1066,11 @@
       <c r="C27" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -992,8 +1080,11 @@
       <c r="C28" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1003,8 +1094,11 @@
       <c r="C29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1014,8 +1108,11 @@
       <c r="C30" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1025,11 +1122,14 @@
       <c r="C31" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1039,8 +1139,11 @@
       <c r="C32" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1050,8 +1153,11 @@
       <c r="C33" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1062,11 +1168,14 @@
         <v>70</v>
       </c>
       <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
+  <sortState ref="A2:D35">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ver_0.2.0_beta_updates - update DB
</commit_message>
<xml_diff>
--- a/resources/db/Case_Types.xlsx
+++ b/resources/db/Case_Types.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python310\MuniEntry\resources\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EE96FFF-44D4-4261-8ED9-AF85A609FD92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,9 +102,6 @@
     <t>4511.29</t>
   </si>
   <si>
-    <t>Space between Moving Vehicles</t>
-  </si>
-  <si>
     <t>4511.34</t>
   </si>
   <si>
@@ -144,9 +147,6 @@
     <t>4510.16</t>
   </si>
   <si>
-    <t>4510.12</t>
-  </si>
-  <si>
     <t>Failure to Reinstate</t>
   </si>
   <si>
@@ -249,9 +249,6 @@
     <t xml:space="preserve">4510.111 </t>
   </si>
   <si>
-    <t>Driving Under Suspension FTA, fines or Child Support</t>
-  </si>
-  <si>
     <t>4510.12(C)(2)</t>
   </si>
   <si>
@@ -271,12 +268,21 @@
   </si>
   <si>
     <t>Criminal</t>
+  </si>
+  <si>
+    <t>4510.21</t>
+  </si>
+  <si>
+    <t>Following Too Close</t>
+  </si>
+  <si>
+    <t>Driving Under Suspension FTA, Fines or Child Support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -309,7 +315,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,8 +343,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,30 +651,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="15.38671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.38671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.38671875" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +685,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -688,125 +694,125 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="D8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
       <c r="D9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -814,47 +820,47 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -862,13 +868,13 @@
         <v>4513.04</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -876,13 +882,13 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -890,131 +896,131 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+      <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1022,114 +1028,114 @@
         <v>4511.21</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1137,27 +1143,27 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1165,20 +1171,20 @@
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E34" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>